<commit_message>
Corregí los psp's de la ClaseConfiguración
</commit_message>
<xml_diff>
--- a/Documentación/Psp's/Axel/Clase Configuración/DefectRemovalEfficiency.xlsx
+++ b/Documentación/Psp's/Axel/Clase Configuración/DefectRemovalEfficiency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AxeelZR\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EE3414A-B289-4176-862F-1907E3FA190C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E44A6D-E526-4FE2-AD10-9508653B9E22}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Adapted from "PSP Materials," copyright © 2006 Carnegie Mellon University. Used by permission.</t>
   </si>
   <si>
-    <t>Reporte generado a las 04:09 PM el 4/12/2018</t>
+    <t>Reporte generado a las 11:24 AM el 5/12/2018</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Correción psp´s  Clase Configuración
</commit_message>
<xml_diff>
--- a/Documentación/Psp's/Axel/Clase Configuración/DefectRemovalEfficiency.xlsx
+++ b/Documentación/Psp's/Axel/Clase Configuración/DefectRemovalEfficiency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AxeelZR\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92E44A6D-E526-4FE2-AD10-9508653B9E22}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8812544D-4303-4F34-BF35-AF11DD425199}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Adapted from "PSP Materials," copyright © 2006 Carnegie Mellon University. Used by permission.</t>
   </si>
   <si>
-    <t>Reporte generado a las 11:24 AM el 5/12/2018</t>
+    <t>Reporte generado a las 01:37 PM el 5/12/2018</t>
   </si>
 </sst>
 </file>

</xml_diff>